<commit_message>
Generate run info for illumina experiment
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/test_services/templates/Experiment_run_MGI_v3_10_0.xlsx
+++ b/backend/fms_core/tests/test_services/templates/Experiment_run_MGI_v3_10_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckostiw/C3G/repos/freezeman/backend/fms_core/tests/test_services/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4603D674-026B-754C-AEC3-5831A6952287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA8355-134F-7D41-8509-534444B8DB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31060" yWindow="5800" windowWidth="30880" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68360" yWindow="-5500" windowWidth="31440" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -1398,7 +1398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1441,6 +1441,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1599,13 +1604,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1823,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1936,11 +1941,11 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -10103,10 +10108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10169,14 +10174,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>446</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>447</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -10256,7 +10261,7 @@
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="6"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -10266,28 +10271,28 @@
       <c r="D16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -17126,63 +17131,36 @@
       <c r="D996" s="2"/>
       <c r="F996" s="2"/>
     </row>
-    <row r="997" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="2"/>
-      <c r="B997" s="2"/>
-      <c r="C997" s="2"/>
-      <c r="D997" s="2"/>
-      <c r="F997" s="2"/>
-    </row>
-    <row r="998" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="2"/>
-      <c r="B998" s="2"/>
-      <c r="C998" s="2"/>
-      <c r="D998" s="2"/>
-      <c r="F998" s="2"/>
-    </row>
-    <row r="999" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="F999" s="2"/>
-    </row>
-    <row r="1000" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="F1000" s="2"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>Index!$C$2:$C$97</xm:f>
-          </x14:formula1>
-          <xm:sqref>D5:D101</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Index!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>F5</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Index!$C$2:$C$97</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D97</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Experiments!$A$11:$A$110</xm:f>
           </x14:formula1>
-          <xm:sqref>A5:A100</xm:sqref>
+          <xm:sqref>A5:A96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Index!$B$2:$B$25</xm:f>
           </x14:formula1>
-          <xm:sqref>F6:F101</xm:sqref>
+          <xm:sqref>F6:F97</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Exercise the two services
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/test_services/templates/Experiment_run_MGI_v3_10_0.xlsx
+++ b/backend/fms_core/tests/test_services/templates/Experiment_run_MGI_v3_10_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckostiw/C3G/repos/freezeman/backend/fms_core/tests/test_services/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FA8355-134F-7D41-8509-534444B8DB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619D7C38-B3CD-7748-AB0D-FCF34A1CF309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68360" yWindow="-5500" windowWidth="31440" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68360" yWindow="-5500" windowWidth="31440" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
             <sz val="11"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>MGI Flowcell Barcode</t>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="449">
   <si>
     <t>Experiment Submission Template</t>
   </si>
@@ -1389,6 +1390,9 @@
   </si>
   <si>
     <t>ER_Container_BC_01</t>
+  </si>
+  <si>
+    <t>Experiment Run Info Test</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1410,41 +1414,55 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1828,8 +1846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2028,7 +2046,9 @@
       <c r="E11" s="11">
         <v>44642</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="11" t="s">
+        <v>448</v>
+      </c>
       <c r="G11" s="2" t="s">
         <v>445</v>
       </c>
@@ -10110,8 +10130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10192,6 +10212,9 @@
       </c>
       <c r="F5" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>